<commit_message>
LAP22G31-138 #comment final Changes
</commit_message>
<xml_diff>
--- a/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
+++ b/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\lapr3-2021-g031\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10775C50-9443-40D5-8716-2F41B2FE5DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE0566-5865-413A-88EC-BF13B5FA4B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -3504,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B77AED-41D5-8047-A901-AF6E531ADCF8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3548,7 +3548,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="64">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D4" s="22">
         <v>80</v>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="F4" s="12">
         <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3569,17 +3569,17 @@
         <v>21</v>
       </c>
       <c r="C5" s="31">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D5" s="7">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E5" s="7">
         <v>85</v>
       </c>
       <c r="F5" s="16">
         <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>-13</v>
       </c>
       <c r="C6" s="30">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -3611,7 +3611,7 @@
         <v>-13</v>
       </c>
       <c r="C7" s="65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="24">
         <v>5</v>
@@ -3636,7 +3636,7 @@
       <c r="E8" s="57"/>
       <c r="F8" s="58">
         <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>46.6</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>0.84727272727272729</v>
+        <v>0.13363636363636364</v>
       </c>
     </row>
   </sheetData>
@@ -3812,67 +3812,67 @@
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>4.2363636363636363</v>
+        <v>0.66818181818181821</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>4.2363636363636354</v>
+        <v>0.6681818181818181</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>60</v>
@@ -4117,63 +4117,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>4.3827272727272728</v>
+        <v>3.1338636363636363</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>4.1577272727272732</v>
+        <v>2.9088636363636362</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>3.9077272727272727</v>
+        <v>2.6588636363636362</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>1.4827272727272727</v>
+        <v>0.23386363636363636</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4192,63 +4192,63 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>17.530909090909091</v>
+        <v>12.535454545454545</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>16.630909090909093</v>
+        <v>11.635454545454545</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>15.630909090909091</v>
+        <v>10.635454545454547</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>5.9309090909090916</v>
+        <v>0.93545454545454543</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -5171,7 +5171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51127868-43C4-0643-A881-5DEA4AEE417A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -5180,6 +5180,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5363,35 +5378,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5413,9 +5403,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
LAP22G31-92 #comment Commit Self-Assement
</commit_message>
<xml_diff>
--- a/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
+++ b/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\lapr3-2021-g031\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE0566-5865-413A-88EC-BF13B5FA4B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F6AA6A-F5CA-4DFE-8177-F64E77C62069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
@@ -3505,7 +3505,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3548,7 +3548,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="64">
-        <v>80</v>
+        <v>80.8</v>
       </c>
       <c r="D4" s="22">
         <v>80</v>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="F4" s="12">
         <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
-        <v>0</v>
+        <v>7.9999999999999707</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3569,7 +3569,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="31">
-        <v>72</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="D5" s="7">
         <v>65</v>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="F5" s="16">
         <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>35</v>
+        <v>32.999999999999972</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>-13</v>
       </c>
       <c r="C6" s="30">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -3636,7 +3636,7 @@
       <c r="E8" s="57"/>
       <c r="F8" s="58">
         <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>7.35</v>
+        <v>9.6499999999999844</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>0.13363636363636364</v>
+        <v>0.17545454545454517</v>
       </c>
     </row>
   </sheetData>
@@ -3812,67 +3812,67 @@
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>0.66818181818181821</v>
+        <v>0.87727272727272587</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>0.6681818181818181</v>
+        <v>0.87727272727272565</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>60</v>
@@ -4117,63 +4117,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>3.1338636363636363</v>
+        <v>3.2070454545454536</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>2.9088636363636362</v>
+        <v>2.982045454545454</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>2.6588636363636362</v>
+        <v>2.732045454545454</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>0.23386363636363636</v>
+        <v>0.30704545454545401</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4192,63 +4192,63 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>12.535454545454545</v>
+        <v>12.828181818181815</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>11.635454545454545</v>
+        <v>11.928181818181816</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>10.635454545454547</v>
+        <v>10.928181818181816</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>0.93545454545454543</v>
+        <v>1.228181818181816</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -5180,21 +5180,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -5378,10 +5363,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5403,19 +5413,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA1CEFC-B112-44A5-8B0C-097F64092DA8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
LAP22G31-134 #comment Self-Assessment done
</commit_message>
<xml_diff>
--- a/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
+++ b/docs/LAPR3-2021-Self-Assessment - Sprint2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\lapr3-2021-g031\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diasd\OneDrive\Documentos\lapr3-2021-g031\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F6AA6A-F5CA-4DFE-8177-F64E77C62069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0357848D-6DB1-4C9D-A7B9-83CAC3949E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1376,7 +1376,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1769,7 +1769,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2067,37 +2067,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.8984375" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>149</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2108,13 +2108,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="78" t="s">
@@ -2136,7 +2136,7 @@
       <c r="S8" s="79"/>
       <c r="T8" s="80"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="45">
@@ -2203,7 +2203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="75">
         <v>1191604</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="76"/>
       <c r="C11" s="8">
         <v>1171444</v>
@@ -2267,17 +2267,29 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="76"/>
       <c r="C12" s="8">
         <v>1190539</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="39">
+        <v>4</v>
+      </c>
+      <c r="G12" s="38">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4</v>
+      </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -2287,12 +2299,12 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="54" t="e">
+      <c r="S12" s="54">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="76"/>
       <c r="C13" s="8">
         <v>1190797</v>
@@ -2317,7 +2329,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="76"/>
       <c r="C14" s="8">
         <v>1190818</v>
@@ -2342,7 +2354,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="76"/>
       <c r="C15" s="8">
         <v>1191604</v>
@@ -2367,7 +2379,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="76"/>
       <c r="C16" s="8" t="s">
         <v>6</v>
@@ -2392,7 +2404,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="76"/>
       <c r="C17" s="8" t="s">
         <v>7</v>
@@ -2417,7 +2429,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="76"/>
       <c r="C18" s="8" t="s">
         <v>8</v>
@@ -2442,7 +2454,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="76"/>
       <c r="C19" s="8" t="s">
         <v>9</v>
@@ -2467,7 +2479,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="76"/>
       <c r="C20" s="8" t="s">
         <v>10</v>
@@ -2492,7 +2504,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="76"/>
       <c r="C21" s="8" t="s">
         <v>11</v>
@@ -2517,7 +2529,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="76"/>
       <c r="C22" s="8" t="s">
         <v>12</v>
@@ -2542,7 +2554,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="76"/>
       <c r="C23" s="8" t="s">
         <v>13</v>
@@ -2567,7 +2579,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="77"/>
       <c r="C24" s="43" t="s">
         <v>14</v>
@@ -2592,7 +2604,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="48" t="s">
         <v>5</v>
@@ -2615,7 +2627,7 @@
       </c>
       <c r="H25" s="49">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I25" s="49">
         <f t="shared" si="1"/>
@@ -2659,27 +2671,27 @@
       </c>
       <c r="S25" s="56"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2687,7 +2699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2695,7 +2707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2703,7 +2715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2711,7 +2723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2719,7 +2731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2746,25 +2758,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="75" t="s">
         <v>26</v>
       </c>
@@ -2796,7 +2808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="76"/>
       <c r="B4" s="84"/>
       <c r="C4" s="84"/>
@@ -2820,7 +2832,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="76"/>
       <c r="B5" s="84"/>
       <c r="C5" s="84"/>
@@ -2844,7 +2856,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>150</v>
       </c>
@@ -2874,7 +2886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>151</v>
       </c>
@@ -2904,7 +2916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>152</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>153</v>
       </c>
@@ -2964,7 +2976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>154</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>155</v>
       </c>
@@ -3024,7 +3036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>156</v>
       </c>
@@ -3054,7 +3066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>157</v>
       </c>
@@ -3084,7 +3096,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>158</v>
       </c>
@@ -3114,7 +3126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>159</v>
       </c>
@@ -3144,7 +3156,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3168,7 +3180,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3192,7 +3204,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3216,7 +3228,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3240,7 +3252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3264,7 +3276,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3288,7 +3300,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -3312,7 +3324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3336,7 +3348,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3360,7 +3372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="23"/>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -3504,23 +3516,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B77AED-41D5-8047-A901-AF6E531ADCF8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="6" width="14.875" customWidth="1"/>
+    <col min="2" max="6" width="14.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>44</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
         <v>50</v>
       </c>
@@ -3561,7 +3573,7 @@
         <v>7.9999999999999707</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="62" t="s">
         <v>51</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>32.999999999999972</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="62" t="s">
         <v>52</v>
       </c>
@@ -3603,7 +3615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="63" t="s">
         <v>53</v>
       </c>
@@ -3624,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="48" t="s">
         <v>54</v>
       </c>
@@ -3639,7 +3651,7 @@
         <v>9.6499999999999844</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="66"/>
       <c r="B9" s="67"/>
       <c r="C9" s="67"/>
@@ -3662,27 +3674,27 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
@@ -3701,8 +3713,8 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>57</v>
       </c>
@@ -3803,7 +3815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>59</v>
       </c>
@@ -3895,7 +3907,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>61</v>
       </c>
@@ -3948,7 +3960,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="16"/>
     </row>
-    <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>68</v>
       </c>
@@ -4001,7 +4013,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>75</v>
       </c>
@@ -4054,7 +4066,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>81</v>
       </c>
@@ -4107,7 +4119,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>55</v>
       </c>
@@ -4185,7 +4197,7 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>87</v>
       </c>
@@ -4260,7 +4272,7 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="17"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>88</v>
       </c>
@@ -4284,22 +4296,22 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>148</v>
       </c>
@@ -4318,7 +4330,7 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>57</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>89</v>
       </c>
@@ -4472,7 +4484,7 @@
       <c r="Y4" s="71"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>96</v>
       </c>
@@ -4525,7 +4537,7 @@
       <c r="Y5" s="71"/>
       <c r="Z5" s="16"/>
     </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -4578,7 +4590,7 @@
       <c r="Y6" s="71"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>110</v>
       </c>
@@ -4631,7 +4643,7 @@
       <c r="Y7" s="71"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>116</v>
       </c>
@@ -4684,7 +4696,7 @@
       <c r="Y8" s="71"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>122</v>
       </c>
@@ -4733,7 +4745,7 @@
       <c r="Y9" s="71"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>127</v>
       </c>
@@ -4786,7 +4798,7 @@
       <c r="Y10" s="71"/>
       <c r="Z10" s="16"/>
     </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>133</v>
       </c>
@@ -4839,7 +4851,7 @@
       <c r="Y11" s="71"/>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>139</v>
       </c>
@@ -4892,7 +4904,7 @@
       <c r="Y12" s="71"/>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>140</v>
       </c>
@@ -4945,7 +4957,7 @@
       <c r="Y13" s="71"/>
       <c r="Z13" s="16"/>
     </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>147</v>
       </c>
@@ -4998,7 +5010,7 @@
       <c r="Y14" s="71"/>
       <c r="Z14" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>55</v>
       </c>
@@ -5076,7 +5088,7 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>87</v>
       </c>
@@ -5151,7 +5163,7 @@
       <c r="Y16" s="24"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>88</v>
       </c>
@@ -5173,7 +5185,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5364,18 +5376,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5397,6 +5409,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5410,12 +5430,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>